<commit_message>
Tidy up handling of config inputs so more user friendly layout can be used
</commit_message>
<xml_diff>
--- a/TestComponents/OtherBits/Copy of Crop Rotation Validation.xlsx
+++ b/TestComponents/OtherBits/Copy of Crop Rotation Validation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1989s\study\LastYear\CAPSTONE\helpfulInfo\svs2\modelCsharp\TestModel\TestModel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\SVSModelBuildDeploy\TestComponents\OtherBits\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0757D3CA-9226-4C8F-AB80-4AD939758027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F57925B8-372F-4E7F-94B8-4659B02563D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D68C7BAB-80DE-42A0-A5F7-D611BF3989D6}"/>
+    <workbookView xWindow="-16320" yWindow="-5925" windowWidth="16440" windowHeight="28440" xr2:uid="{D68C7BAB-80DE-42A0-A5F7-D611BF3989D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Lovett" sheetId="1" r:id="rId1"/>
@@ -98,7 +98,7 @@
     Assuming good moisture 0-15 cm</t>
       </text>
     </comment>
-    <comment ref="C33" authorId="6" shapeId="0" xr:uid="{CC4D6E8B-A0AF-4A8D-ADFE-33058901246C}">
+    <comment ref="C30" authorId="6" shapeId="0" xr:uid="{CC4D6E8B-A0AF-4A8D-ADFE-33058901246C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -106,7 +106,7 @@
     @ 14% moisture - not specified in the tool</t>
       </text>
     </comment>
-    <comment ref="D33" authorId="7" shapeId="0" xr:uid="{4A24CD7E-B336-4CA9-8481-C31D95EDC06A}">
+    <comment ref="D30" authorId="7" shapeId="0" xr:uid="{4A24CD7E-B336-4CA9-8481-C31D95EDC06A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -114,7 +114,7 @@
     @ 14% moisture</t>
       </text>
     </comment>
-    <comment ref="C50" authorId="8" shapeId="0" xr:uid="{41971706-E29E-4BB2-BCA0-94F2423467A9}">
+    <comment ref="C44" authorId="8" shapeId="0" xr:uid="{41971706-E29E-4BB2-BCA0-94F2423467A9}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -244,7 +244,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="101">
   <si>
     <t>Property</t>
   </si>
@@ -1117,13 +1117,13 @@
   <threadedComment ref="C19" dT="2023-10-26T01:15:36.57" personId="{2BEBAB2E-91BA-40B3-BEE5-7E6784164FBF}" id="{B9626CDC-644A-49BA-B1FD-6B5F8316418E}">
     <text>Assuming good moisture 0-15 cm</text>
   </threadedComment>
-  <threadedComment ref="C33" dT="2023-10-26T01:20:47.03" personId="{2BEBAB2E-91BA-40B3-BEE5-7E6784164FBF}" id="{CC4D6E8B-A0AF-4A8D-ADFE-33058901246C}">
+  <threadedComment ref="C30" dT="2023-10-26T01:20:47.03" personId="{2BEBAB2E-91BA-40B3-BEE5-7E6784164FBF}" id="{CC4D6E8B-A0AF-4A8D-ADFE-33058901246C}">
     <text>@ 14% moisture - not specified in the tool</text>
   </threadedComment>
-  <threadedComment ref="D33" dT="2023-10-26T01:34:32.50" personId="{2BEBAB2E-91BA-40B3-BEE5-7E6784164FBF}" id="{4A24CD7E-B336-4CA9-8481-C31D95EDC06A}">
+  <threadedComment ref="D30" dT="2023-10-26T01:34:32.50" personId="{2BEBAB2E-91BA-40B3-BEE5-7E6784164FBF}" id="{4A24CD7E-B336-4CA9-8481-C31D95EDC06A}">
     <text>@ 14% moisture</text>
   </threadedComment>
-  <threadedComment ref="C50" dT="2023-10-26T01:34:32.50" personId="{2BEBAB2E-91BA-40B3-BEE5-7E6784164FBF}" id="{41971706-E29E-4BB2-BCA0-94F2423467A9}">
+  <threadedComment ref="C44" dT="2023-10-26T01:34:32.50" personId="{2BEBAB2E-91BA-40B3-BEE5-7E6784164FBF}" id="{41971706-E29E-4BB2-BCA0-94F2423467A9}">
     <text>@ 14% moisture</text>
   </threadedComment>
 </ThreadedComments>
@@ -1172,19 +1172,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C27FB4FB-42CF-4046-81E6-EAE466E39234}">
-  <dimension ref="A1:V66"/>
+  <dimension ref="A1:V57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="L43" sqref="L43"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="24.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -1213,7 +1213,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
@@ -1242,7 +1242,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>1.31</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -1270,7 +1270,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>8</v>
@@ -1299,7 +1299,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>9</v>
@@ -1314,7 +1314,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>10</v>
@@ -1329,7 +1329,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>11</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>12</v>
@@ -1358,7 +1358,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>14</v>
@@ -1372,8 +1372,26 @@
       <c r="E13" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G13" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="H13" s="12"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="5"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
         <v>16</v>
@@ -1387,8 +1405,26 @@
       <c r="E14" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G14" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7"/>
+      <c r="U14" s="7"/>
+      <c r="V14" s="8"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>78</v>
       </c>
@@ -1404,8 +1440,26 @@
       <c r="E15" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G15" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="7"/>
+      <c r="V15" s="8"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="19"/>
       <c r="B16" t="s">
         <v>19</v>
@@ -1419,8 +1473,26 @@
       <c r="E16">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="G16" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
+      <c r="U16" s="7"/>
+      <c r="V16" s="8"/>
+    </row>
+    <row r="17" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="19"/>
       <c r="B17" s="1" t="s">
         <v>20</v>
@@ -1434,8 +1506,26 @@
       <c r="E17" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="G17" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="9"/>
+      <c r="V17" s="10"/>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
       <c r="B18" s="1" t="s">
         <v>21</v>
@@ -1450,7 +1540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="19"/>
       <c r="B19" t="s">
         <v>22</v>
@@ -1465,7 +1555,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="19"/>
       <c r="B20" s="2" t="s">
         <v>23</v>
@@ -1479,832 +1569,580 @@
       <c r="E20" s="3">
         <v>44831</v>
       </c>
-      <c r="G20" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="H20" s="12"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
-      <c r="T20" s="4"/>
-      <c r="U20" s="4"/>
-      <c r="V20" s="5"/>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="19"/>
-      <c r="B21" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="2">
-        <f t="shared" ref="C21" si="0">YEAR(C20)</f>
-        <v>2020</v>
-      </c>
-      <c r="D21" s="2">
-        <f t="shared" ref="D21" si="1">YEAR(D20)</f>
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A22" s="19"/>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="3">
+        <v>44272</v>
+      </c>
+      <c r="D22" s="3">
+        <v>44587</v>
+      </c>
+      <c r="E22" s="3">
+        <v>44951</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23" s="19"/>
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23">
         <v>2021</v>
       </c>
-      <c r="E21" s="2">
-        <f>YEAR(E20)</f>
+      <c r="D23">
         <v>2022</v>
       </c>
-      <c r="G21" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
-      <c r="Q21" s="7"/>
-      <c r="R21" s="7"/>
-      <c r="S21" s="7"/>
-      <c r="T21" s="7"/>
-      <c r="U21" s="7"/>
-      <c r="V21" s="8"/>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A22" s="19"/>
-      <c r="B22" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="2">
-        <f t="shared" ref="C22:D22" si="2">MONTH(C20)</f>
-        <v>9</v>
-      </c>
-      <c r="D22" s="2">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="E22" s="2">
-        <f>MONTH(E20)</f>
-        <v>9</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="7"/>
-      <c r="P22" s="7"/>
-      <c r="Q22" s="7"/>
-      <c r="R22" s="7"/>
-      <c r="S22" s="7"/>
-      <c r="T22" s="7"/>
-      <c r="U22" s="7"/>
-      <c r="V22" s="8"/>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A23" s="19"/>
-      <c r="B23" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="2">
-        <f t="shared" ref="C23:D23" si="3">DAY(C20)</f>
-        <v>24</v>
-      </c>
-      <c r="D23" s="2">
-        <f t="shared" si="3"/>
-        <v>21</v>
-      </c>
-      <c r="E23" s="2">
-        <f>DAY(E20)</f>
-        <v>27</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7"/>
-      <c r="O23" s="7"/>
-      <c r="P23" s="7"/>
-      <c r="Q23" s="7"/>
-      <c r="R23" s="7"/>
-      <c r="S23" s="7"/>
-      <c r="T23" s="7"/>
-      <c r="U23" s="7"/>
-      <c r="V23" s="8"/>
-    </row>
-    <row r="24" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E23">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
       <c r="B24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" t="s">
-        <v>28</v>
-      </c>
-      <c r="E24" t="s">
-        <v>28</v>
-      </c>
-      <c r="G24" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="9"/>
-      <c r="P24" s="9"/>
-      <c r="Q24" s="9"/>
-      <c r="R24" s="9"/>
-      <c r="S24" s="9"/>
-      <c r="T24" s="9"/>
-      <c r="U24" s="9"/>
-      <c r="V24" s="10"/>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="19"/>
       <c r="B25" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" s="3">
-        <v>44272</v>
-      </c>
-      <c r="D25" s="3">
-        <v>44587</v>
-      </c>
-      <c r="E25" s="3">
-        <v>44951</v>
-      </c>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+      <c r="C25">
+        <v>21</v>
+      </c>
+      <c r="D25">
+        <v>26</v>
+      </c>
+      <c r="E25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>
       <c r="B26" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26">
-        <v>2021</v>
-      </c>
-      <c r="D26">
-        <v>2022</v>
-      </c>
-      <c r="E26">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+      <c r="C26" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" t="s">
+        <v>82</v>
+      </c>
+      <c r="E26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
       <c r="B27" t="s">
-        <v>31</v>
-      </c>
-      <c r="C27">
-        <v>3</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="C27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" t="s">
+        <v>100</v>
+      </c>
+      <c r="E27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="19"/>
       <c r="B28" t="s">
-        <v>32</v>
-      </c>
-      <c r="C28">
-        <v>21</v>
-      </c>
-      <c r="D28">
-        <v>26</v>
-      </c>
-      <c r="E28">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A29" s="19"/>
-      <c r="B29" t="s">
-        <v>33</v>
-      </c>
-      <c r="C29" t="s">
-        <v>55</v>
-      </c>
-      <c r="D29" t="s">
-        <v>82</v>
-      </c>
-      <c r="E29" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A30" s="19"/>
+        <v>37</v>
+      </c>
+      <c r="C28" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A30" s="21"/>
       <c r="B30" t="s">
-        <v>35</v>
-      </c>
-      <c r="C30" t="s">
-        <v>36</v>
-      </c>
-      <c r="D30" t="s">
-        <v>100</v>
-      </c>
-      <c r="E30" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="31" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="19"/>
-      <c r="B31" t="s">
-        <v>37</v>
-      </c>
-      <c r="C31" t="s">
-        <v>38</v>
-      </c>
-      <c r="D31" t="s">
-        <v>38</v>
-      </c>
-      <c r="E31" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="32" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="B32" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="C32" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="D32" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="E32" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+      <c r="C30">
+        <v>12.7</v>
+      </c>
+      <c r="D30">
+        <v>4.7</v>
+      </c>
+      <c r="E30" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A31" s="21"/>
+      <c r="B31" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A32" s="21"/>
+      <c r="B32" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0</v>
+      </c>
+      <c r="E32" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="21"/>
       <c r="B33" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C33">
-        <v>12.7</v>
+        <v>30</v>
       </c>
       <c r="D33">
-        <v>4.7</v>
-      </c>
-      <c r="E33" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+      <c r="E33">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="21"/>
-      <c r="B34" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C34" s="1">
-        <v>0</v>
-      </c>
-      <c r="D34" s="1">
-        <v>0</v>
-      </c>
-      <c r="E34" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B34" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" s="3">
+        <v>44307</v>
+      </c>
+      <c r="D34" s="3">
+        <v>44831</v>
+      </c>
+      <c r="E34" s="3">
+        <v>45026</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="21"/>
-      <c r="B35" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C35" s="1">
-        <v>0</v>
-      </c>
-      <c r="D35" s="1">
-        <v>0</v>
-      </c>
-      <c r="E35" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D35" t="s">
+        <v>28</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="21"/>
       <c r="B36" t="s">
-        <v>44</v>
-      </c>
-      <c r="C36">
-        <v>30</v>
-      </c>
-      <c r="D36">
-        <v>30</v>
-      </c>
-      <c r="E36">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+      <c r="C36" s="3">
+        <v>44587</v>
+      </c>
+      <c r="D36" s="3">
+        <v>44951</v>
+      </c>
+      <c r="E36" s="15">
+        <v>45142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="21"/>
-      <c r="B37" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C37" s="3">
-        <v>44307</v>
-      </c>
-      <c r="D37" s="3">
-        <v>44831</v>
-      </c>
-      <c r="E37" s="3">
-        <v>45026</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>51</v>
+      </c>
+      <c r="C37">
+        <v>2022</v>
+      </c>
+      <c r="D37">
+        <v>2023</v>
+      </c>
+      <c r="E37" s="2">
+        <f>YEAR(E36)</f>
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="21"/>
-      <c r="B38" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C38" s="2">
-        <f t="shared" ref="C38:D38" si="4">YEAR(C37)</f>
-        <v>2021</v>
-      </c>
-      <c r="D38" s="2">
-        <f t="shared" si="4"/>
-        <v>2022</v>
+      <c r="B38" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
       </c>
       <c r="E38" s="2">
-        <f>YEAR(E37)</f>
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+        <f>MONTH(E36)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="21"/>
-      <c r="B39" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C39" s="2">
-        <f t="shared" ref="C39:D39" si="5">MONTH(C37)</f>
+      <c r="B39" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39">
+        <v>26</v>
+      </c>
+      <c r="D39">
+        <v>25</v>
+      </c>
+      <c r="E39" s="2">
+        <f>DAY(E36)</f>
         <v>4</v>
       </c>
-      <c r="D39" s="2">
-        <f t="shared" si="5"/>
-        <v>9</v>
-      </c>
-      <c r="E39" s="2">
-        <f>MONTH(E37)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="21"/>
-      <c r="B40" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C40" s="2">
-        <f t="shared" ref="C40:D40" si="6">DAY(C37)</f>
-        <v>21</v>
-      </c>
-      <c r="D40" s="2">
-        <f t="shared" si="6"/>
-        <v>27</v>
-      </c>
-      <c r="E40" s="2">
-        <f>DAY(E37)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
+        <v>54</v>
+      </c>
+      <c r="C40" t="s">
+        <v>82</v>
+      </c>
+      <c r="D40" t="s">
+        <v>82</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="21"/>
       <c r="B41" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C41" t="s">
+        <v>100</v>
+      </c>
+      <c r="D41" t="s">
+        <v>36</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="22"/>
+      <c r="B42" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E42" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C43" t="s">
+        <v>84</v>
+      </c>
+      <c r="D43" t="s">
+        <v>59</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="23"/>
+      <c r="B44" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C44">
+        <v>4.7</v>
+      </c>
+      <c r="D44" s="2">
+        <v>10</v>
+      </c>
+      <c r="E44" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="23"/>
+      <c r="B45" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C45" s="1">
+        <v>0</v>
+      </c>
+      <c r="D45" s="2">
+        <v>0</v>
+      </c>
+      <c r="E45" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="23"/>
+      <c r="B46" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" s="1">
+        <v>0</v>
+      </c>
+      <c r="D46" s="2">
+        <v>0</v>
+      </c>
+      <c r="E46" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="23"/>
+      <c r="B47" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C47">
+        <v>30</v>
+      </c>
+      <c r="D47">
+        <v>40</v>
+      </c>
+      <c r="E47" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="23"/>
+      <c r="B48" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C48" s="3">
+        <v>44831</v>
+      </c>
+      <c r="D48" s="3">
+        <v>45026</v>
+      </c>
+      <c r="E48" s="15">
+        <v>45170</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="23"/>
+      <c r="B49" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C49" t="s">
         <v>28</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D49" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="E49" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="21"/>
-      <c r="B42" t="s">
-        <v>50</v>
-      </c>
-      <c r="C42" s="3">
-        <v>44587</v>
-      </c>
-      <c r="D42" s="3">
-        <v>44951</v>
-      </c>
-      <c r="E42" s="15">
-        <v>45142</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="21"/>
-      <c r="B43" t="s">
-        <v>51</v>
-      </c>
-      <c r="C43">
-        <v>2022</v>
-      </c>
-      <c r="D43">
-        <v>2023</v>
-      </c>
-      <c r="E43" s="2">
-        <f>YEAR(E42)</f>
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" s="21"/>
-      <c r="B44" t="s">
-        <v>52</v>
-      </c>
-      <c r="C44">
-        <v>1</v>
-      </c>
-      <c r="D44">
-        <v>1</v>
-      </c>
-      <c r="E44" s="2">
-        <f>MONTH(E42)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="21"/>
-      <c r="B45" t="s">
-        <v>53</v>
-      </c>
-      <c r="C45">
-        <v>26</v>
-      </c>
-      <c r="D45">
-        <v>25</v>
-      </c>
-      <c r="E45" s="2">
-        <f>DAY(E42)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="21"/>
-      <c r="B46" t="s">
-        <v>54</v>
-      </c>
-      <c r="C46" t="s">
-        <v>82</v>
-      </c>
-      <c r="D46" t="s">
-        <v>82</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="21"/>
-      <c r="B47" t="s">
-        <v>56</v>
-      </c>
-      <c r="C47" t="s">
-        <v>100</v>
-      </c>
-      <c r="D47" t="s">
-        <v>36</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="22"/>
-      <c r="B48" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="C48" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D48" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="E48" s="18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C49" t="s">
-        <v>84</v>
-      </c>
-      <c r="D49" t="s">
-        <v>59</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="23"/>
       <c r="B50" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C50">
-        <v>4.7</v>
-      </c>
-      <c r="D50" s="2">
-        <v>10</v>
-      </c>
-      <c r="E50" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+      <c r="C50" s="3">
+        <v>44951</v>
+      </c>
+      <c r="D50" s="15">
+        <v>45142</v>
+      </c>
+      <c r="E50" s="15">
+        <v>45200</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="23"/>
       <c r="B51" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C51" s="1">
-        <v>0</v>
+        <v>70</v>
+      </c>
+      <c r="C51">
+        <v>2023</v>
       </c>
       <c r="D51" s="2">
-        <v>0</v>
+        <f>YEAR(D50)</f>
+        <v>2023</v>
       </c>
       <c r="E51" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+        <f>YEAR(E50)</f>
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="23"/>
       <c r="B52" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C52" s="1">
-        <v>0</v>
+        <v>71</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
       </c>
       <c r="D52" s="2">
-        <v>0</v>
+        <f>MONTH(D50)</f>
+        <v>8</v>
       </c>
       <c r="E52" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+        <f>MONTH(E50)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="23"/>
       <c r="B53" s="1" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C53">
-        <v>30</v>
-      </c>
-      <c r="D53">
-        <v>40</v>
+        <v>25</v>
+      </c>
+      <c r="D53" s="2">
+        <f>DAY(D50)</f>
+        <v>4</v>
       </c>
       <c r="E53" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+        <f>DAY(E50)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="23"/>
       <c r="B54" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C54" s="3">
-        <v>44831</v>
-      </c>
-      <c r="D54" s="3">
-        <v>45026</v>
-      </c>
-      <c r="E54" s="15">
-        <v>45170</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+        <v>73</v>
+      </c>
+      <c r="C54" t="s">
+        <v>82</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="23"/>
       <c r="B55" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C55" s="2">
-        <f t="shared" ref="C55" si="7">YEAR(C54)</f>
-        <v>2022</v>
-      </c>
-      <c r="D55" s="2">
-        <f>YEAR(D54)</f>
-        <v>2023</v>
-      </c>
-      <c r="E55" s="2">
-        <f>YEAR(E54)</f>
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+      <c r="C55" t="s">
+        <v>36</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="23"/>
       <c r="B56" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C56" s="2">
-        <f t="shared" ref="C56" si="8">MONTH(C54)</f>
-        <v>9</v>
-      </c>
-      <c r="D56" s="2">
-        <f>MONTH(D54)</f>
-        <v>4</v>
-      </c>
-      <c r="E56" s="2">
-        <f>MONTH(E54)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" s="23"/>
+        <v>75</v>
+      </c>
+      <c r="C56" t="s">
+        <v>38</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="1"/>
       <c r="B57" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C57" s="2">
-        <f t="shared" ref="C57" si="9">DAY(C54)</f>
-        <v>27</v>
-      </c>
-      <c r="D57" s="2">
-        <f>DAY(D54)</f>
-        <v>10</v>
-      </c>
-      <c r="E57" s="2">
-        <f>DAY(E54)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A58" s="23"/>
-      <c r="B58" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C58" t="s">
-        <v>28</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A59" s="23"/>
-      <c r="B59" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C59" s="3">
-        <v>44951</v>
-      </c>
-      <c r="D59" s="15">
-        <v>45142</v>
-      </c>
-      <c r="E59" s="15">
-        <v>45200</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A60" s="23"/>
-      <c r="B60" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C60">
-        <v>2023</v>
-      </c>
-      <c r="D60" s="2">
-        <f>YEAR(D59)</f>
-        <v>2023</v>
-      </c>
-      <c r="E60" s="2">
-        <f>YEAR(E59)</f>
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A61" s="23"/>
-      <c r="B61" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C61">
-        <v>1</v>
-      </c>
-      <c r="D61" s="2">
-        <f>MONTH(D59)</f>
-        <v>8</v>
-      </c>
-      <c r="E61" s="2">
-        <f>MONTH(E59)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A62" s="23"/>
-      <c r="B62" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C62">
-        <v>25</v>
-      </c>
-      <c r="D62" s="2">
-        <f>DAY(D59)</f>
-        <v>4</v>
-      </c>
-      <c r="E62" s="2">
-        <f>DAY(E59)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A63" s="23"/>
-      <c r="B63" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C63" t="s">
-        <v>82</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A64" s="23"/>
-      <c r="B64" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C64" t="s">
-        <v>36</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A65" s="23"/>
-      <c r="B65" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C65" t="s">
-        <v>38</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C57" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="D57" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E66" s="1" t="s">
+      <c r="E57" s="1" t="s">
         <v>77</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A15:A31"/>
-    <mergeCell ref="A32:A48"/>
-    <mergeCell ref="A49:A65"/>
+    <mergeCell ref="A15:A28"/>
+    <mergeCell ref="A29:A42"/>
+    <mergeCell ref="A43:A56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -2319,14 +2157,14 @@
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.453125" customWidth="1"/>
-    <col min="4" max="5" width="24.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="5" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2340,7 +2178,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -2355,7 +2193,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -2369,7 +2207,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
@@ -2384,7 +2222,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -2398,7 +2236,7 @@
         <v>1.27</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -2412,7 +2250,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
@@ -2420,7 +2258,7 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>8</v>
@@ -2435,7 +2273,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>9</v>
@@ -2450,7 +2288,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>10</v>
@@ -2465,7 +2303,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>11</v>
       </c>
@@ -2479,7 +2317,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>12</v>
@@ -2494,7 +2332,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>14</v>
@@ -2509,7 +2347,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
         <v>16</v>
@@ -2524,7 +2362,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>78</v>
       </c>
@@ -2541,7 +2379,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="19"/>
       <c r="B16" t="s">
         <v>19</v>
@@ -2556,7 +2394,7 @@
         <v>18.8</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
       <c r="B17" s="1" t="s">
         <v>20</v>
@@ -2571,7 +2409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
       <c r="B18" s="1" t="s">
         <v>21</v>
@@ -2586,7 +2424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="19"/>
       <c r="B19" t="s">
         <v>22</v>
@@ -2601,7 +2439,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="19"/>
       <c r="B20" s="2" t="s">
         <v>23</v>
@@ -2622,7 +2460,7 @@
       <c r="O20" s="4"/>
       <c r="P20" s="5"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="19"/>
       <c r="B21" s="2" t="s">
         <v>24</v>
@@ -2643,7 +2481,7 @@
       <c r="O21" s="7"/>
       <c r="P21" s="8"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="19"/>
       <c r="B22" s="2" t="s">
         <v>25</v>
@@ -2664,7 +2502,7 @@
       <c r="O22" s="7"/>
       <c r="P22" s="8"/>
     </row>
-    <row r="23" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="19"/>
       <c r="B23" s="2" t="s">
         <v>26</v>
@@ -2685,7 +2523,7 @@
       <c r="O23" s="9"/>
       <c r="P23" s="10"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
       <c r="B24" t="s">
         <v>27</v>
@@ -2700,7 +2538,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="19"/>
       <c r="B25" t="s">
         <v>29</v>
@@ -2715,7 +2553,7 @@
         <v>45001</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>
       <c r="B26" t="s">
         <v>30</v>
@@ -2730,7 +2568,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
       <c r="B27" t="s">
         <v>31</v>
@@ -2745,7 +2583,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="19"/>
       <c r="B28" t="s">
         <v>32</v>
@@ -2760,7 +2598,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="19"/>
       <c r="B29" t="s">
         <v>33</v>
@@ -2775,7 +2613,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="19"/>
       <c r="B30" t="s">
         <v>35</v>
@@ -2790,7 +2628,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="19"/>
       <c r="B31" t="s">
         <v>37</v>
@@ -2805,7 +2643,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
         <v>79</v>
       </c>
@@ -2819,7 +2657,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="19"/>
       <c r="B33" t="s">
         <v>41</v>
@@ -2831,7 +2669,7 @@
         <v>18.8</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="19"/>
       <c r="B34" s="13" t="s">
         <v>42</v>
@@ -2844,7 +2682,7 @@
       </c>
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="19"/>
       <c r="B35" s="13" t="s">
         <v>43</v>
@@ -2857,7 +2695,7 @@
       </c>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="19"/>
       <c r="B36" t="s">
         <v>44</v>
@@ -2869,7 +2707,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="19"/>
       <c r="B37" s="2" t="s">
         <v>45</v>
@@ -2878,7 +2716,7 @@
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="19"/>
       <c r="B38" s="2" t="s">
         <v>46</v>
@@ -2887,7 +2725,7 @@
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="19"/>
       <c r="B39" s="2" t="s">
         <v>47</v>
@@ -2896,7 +2734,7 @@
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="19"/>
       <c r="B40" s="2" t="s">
         <v>48</v>
@@ -2905,7 +2743,7 @@
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="19"/>
       <c r="B41" t="s">
         <v>49</v>
@@ -2917,7 +2755,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="19"/>
       <c r="B42" t="s">
         <v>50</v>
@@ -2929,7 +2767,7 @@
         <v>45001</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="19"/>
       <c r="B43" t="s">
         <v>51</v>
@@ -2941,7 +2779,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="19"/>
       <c r="B44" t="s">
         <v>52</v>
@@ -2953,7 +2791,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="19"/>
       <c r="B45" t="s">
         <v>53</v>
@@ -2965,7 +2803,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="19"/>
       <c r="B46" t="s">
         <v>54</v>
@@ -2977,7 +2815,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="19"/>
       <c r="B47" t="s">
         <v>56</v>
@@ -2989,7 +2827,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="19"/>
       <c r="B48" t="s">
         <v>57</v>
@@ -3001,7 +2839,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="23" t="s">
         <v>80</v>
       </c>
@@ -3015,7 +2853,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="23"/>
       <c r="B50" s="1" t="s">
         <v>60</v>
@@ -3030,7 +2868,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="23"/>
       <c r="B51" s="1" t="s">
         <v>61</v>
@@ -3045,7 +2883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="23"/>
       <c r="B52" s="1" t="s">
         <v>62</v>
@@ -3060,7 +2898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="23"/>
       <c r="B53" s="1" t="s">
         <v>63</v>
@@ -3075,7 +2913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="23"/>
       <c r="B54" s="1" t="s">
         <v>64</v>
@@ -3084,7 +2922,7 @@
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="23"/>
       <c r="B55" s="1" t="s">
         <v>65</v>
@@ -3099,7 +2937,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="23"/>
       <c r="B56" s="1" t="s">
         <v>66</v>
@@ -3114,7 +2952,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="23"/>
       <c r="B57" s="1" t="s">
         <v>67</v>
@@ -3129,7 +2967,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="23"/>
       <c r="B58" s="1" t="s">
         <v>68</v>
@@ -3144,7 +2982,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="23"/>
       <c r="B59" s="1" t="s">
         <v>69</v>
@@ -3153,7 +2991,7 @@
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="23"/>
       <c r="B60" s="1" t="s">
         <v>70</v>
@@ -3168,7 +3006,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="23"/>
       <c r="B61" s="1" t="s">
         <v>71</v>
@@ -3183,7 +3021,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="23"/>
       <c r="B62" s="1" t="s">
         <v>72</v>
@@ -3198,7 +3036,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="23"/>
       <c r="B63" s="1" t="s">
         <v>73</v>
@@ -3213,7 +3051,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="23"/>
       <c r="B64" s="1" t="s">
         <v>74</v>
@@ -3228,7 +3066,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="23"/>
       <c r="B65" s="1" t="s">
         <v>75</v>
@@ -3243,7 +3081,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1" t="s">
         <v>76</v>

</xml_diff>